<commit_message>
Improve phrase type determination and remove quick test
Excel_Generator.py now prioritizes the 'type' field from the parser when determining phrase type, falling back to legacy logic if unavailable. Removed quick_test.py as it is no longer needed. Updated the Excel data file.
</commit_message>
<xml_diff>
--- a/training/data/例文入力元_分解結果_v2.xlsx
+++ b/training/data/例文入力元_分解結果_v2.xlsx
@@ -526,7 +526,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -606,7 +606,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -646,7 +646,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -686,7 +686,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -730,7 +730,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -770,7 +770,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -810,7 +810,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -854,7 +854,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -894,7 +894,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
@@ -934,7 +934,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -978,7 +978,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -1678,7 +1678,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H33" t="inlineStr"/>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H34" t="inlineStr"/>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H36" t="inlineStr"/>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H40" t="inlineStr"/>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H41" t="inlineStr"/>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
@@ -2222,7 +2222,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H43" t="inlineStr"/>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H44" t="inlineStr"/>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H45" t="inlineStr"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
@@ -2470,7 +2470,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
@@ -2510,7 +2510,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
@@ -2554,7 +2554,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H51" t="inlineStr"/>
@@ -2594,7 +2594,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H54" t="inlineStr"/>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H55" t="inlineStr"/>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
@@ -3042,7 +3042,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
@@ -3082,7 +3082,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H64" t="inlineStr"/>
@@ -3122,7 +3122,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H65" t="inlineStr"/>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
@@ -3326,7 +3326,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
@@ -3534,7 +3534,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
@@ -3618,7 +3618,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
@@ -3658,7 +3658,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
@@ -3742,7 +3742,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
@@ -3906,7 +3906,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
@@ -3946,7 +3946,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
@@ -4070,7 +4070,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
@@ -4190,7 +4190,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
@@ -4274,7 +4274,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
@@ -4354,7 +4354,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
@@ -4478,7 +4478,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
@@ -4518,7 +4518,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
@@ -4558,7 +4558,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
@@ -4598,7 +4598,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H102" t="inlineStr"/>
@@ -4682,7 +4682,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
@@ -4722,7 +4722,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
@@ -4762,7 +4762,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
@@ -4806,7 +4806,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H106" t="inlineStr"/>
@@ -4846,7 +4846,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H107" t="inlineStr"/>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
@@ -4970,7 +4970,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H110" t="inlineStr"/>
@@ -5010,7 +5010,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H111" t="inlineStr"/>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H112" t="inlineStr"/>
@@ -5094,7 +5094,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H113" t="inlineStr"/>
@@ -5134,7 +5134,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H114" t="inlineStr"/>
@@ -5178,7 +5178,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H115" t="inlineStr"/>
@@ -5218,7 +5218,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H116" t="inlineStr"/>
@@ -5258,7 +5258,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H117" t="inlineStr"/>
@@ -5302,7 +5302,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H118" t="inlineStr"/>
@@ -5342,7 +5342,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H119" t="inlineStr"/>
@@ -5382,7 +5382,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H120" t="inlineStr"/>
@@ -5426,7 +5426,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H121" t="inlineStr"/>
@@ -5466,7 +5466,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H122" t="inlineStr"/>
@@ -5506,7 +5506,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H123" t="inlineStr"/>
@@ -5550,7 +5550,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H124" t="inlineStr"/>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H125" t="inlineStr"/>
@@ -5630,7 +5630,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H126" t="inlineStr"/>
@@ -5674,7 +5674,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H127" t="inlineStr"/>
@@ -5714,7 +5714,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H128" t="inlineStr"/>
@@ -5754,7 +5754,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H129" t="inlineStr"/>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H130" t="inlineStr"/>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H131" t="inlineStr"/>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H132" t="inlineStr"/>
@@ -5918,7 +5918,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H133" t="inlineStr"/>
@@ -5958,7 +5958,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H134" t="inlineStr"/>
@@ -5998,7 +5998,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H135" t="inlineStr"/>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H136" t="inlineStr"/>
@@ -6082,7 +6082,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H137" t="inlineStr"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H138" t="inlineStr"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H139" t="inlineStr"/>
@@ -6202,7 +6202,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H140" t="inlineStr"/>
@@ -6242,7 +6242,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H141" t="inlineStr"/>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H142" t="inlineStr"/>
@@ -6326,7 +6326,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H143" t="inlineStr"/>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H144" t="inlineStr"/>
@@ -6406,7 +6406,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H145" t="inlineStr"/>
@@ -6446,7 +6446,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H146" t="inlineStr"/>
@@ -6490,7 +6490,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H147" t="inlineStr"/>
@@ -6530,7 +6530,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H148" t="inlineStr"/>
@@ -6570,7 +6570,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H149" t="inlineStr"/>
@@ -6614,7 +6614,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H150" t="inlineStr"/>
@@ -6654,7 +6654,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H151" t="inlineStr"/>
@@ -6694,7 +6694,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H152" t="inlineStr"/>
@@ -6738,7 +6738,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H153" t="inlineStr"/>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H154" t="inlineStr"/>
@@ -6818,7 +6818,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H155" t="inlineStr"/>
@@ -6862,7 +6862,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H156" t="inlineStr"/>
@@ -6902,7 +6902,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H157" t="inlineStr"/>
@@ -6942,7 +6942,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H158" t="inlineStr"/>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H159" t="inlineStr"/>
@@ -7026,7 +7026,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H160" t="inlineStr"/>
@@ -7066,7 +7066,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H161" t="inlineStr"/>
@@ -7110,7 +7110,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H162" t="inlineStr"/>
@@ -7150,7 +7150,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H163" t="inlineStr"/>
@@ -7190,7 +7190,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H164" t="inlineStr"/>
@@ -7234,7 +7234,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H165" t="inlineStr"/>
@@ -7274,7 +7274,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H166" t="inlineStr"/>
@@ -7314,7 +7314,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H167" t="inlineStr"/>
@@ -7358,7 +7358,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H168" t="inlineStr"/>
@@ -7398,7 +7398,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H169" t="inlineStr"/>
@@ -7438,7 +7438,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H170" t="inlineStr"/>
@@ -7482,7 +7482,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H171" t="inlineStr"/>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H172" t="inlineStr"/>
@@ -7562,7 +7562,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H173" t="inlineStr"/>
@@ -7606,7 +7606,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H174" t="inlineStr"/>
@@ -7646,7 +7646,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H175" t="inlineStr"/>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H176" t="inlineStr"/>
@@ -7730,7 +7730,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H177" t="inlineStr"/>
@@ -7770,7 +7770,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H178" t="inlineStr"/>
@@ -7810,7 +7810,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H179" t="inlineStr"/>
@@ -7854,7 +7854,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H180" t="inlineStr"/>
@@ -7894,7 +7894,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H181" t="inlineStr"/>
@@ -7934,7 +7934,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H182" t="inlineStr"/>
@@ -7978,7 +7978,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H183" t="inlineStr"/>
@@ -8018,7 +8018,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H184" t="inlineStr"/>
@@ -8058,7 +8058,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H185" t="inlineStr"/>
@@ -8102,7 +8102,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H186" t="inlineStr"/>
@@ -8142,7 +8142,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H187" t="inlineStr"/>
@@ -8182,7 +8182,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H188" t="inlineStr"/>
@@ -8226,7 +8226,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H189" t="inlineStr"/>
@@ -8266,7 +8266,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H190" t="inlineStr"/>
@@ -8306,7 +8306,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H191" t="inlineStr"/>
@@ -8350,7 +8350,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H192" t="inlineStr"/>
@@ -8390,7 +8390,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H193" t="inlineStr"/>
@@ -8430,7 +8430,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H194" t="inlineStr"/>
@@ -8474,7 +8474,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H195" t="inlineStr"/>
@@ -8514,7 +8514,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H196" t="inlineStr"/>
@@ -8554,7 +8554,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H197" t="inlineStr"/>
@@ -8598,7 +8598,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H198" t="inlineStr"/>
@@ -8638,7 +8638,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H199" t="inlineStr"/>
@@ -8678,7 +8678,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H200" t="inlineStr"/>
@@ -8722,7 +8722,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H201" t="inlineStr"/>
@@ -8762,7 +8762,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H202" t="inlineStr"/>
@@ -8802,7 +8802,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H203" t="inlineStr"/>
@@ -8846,7 +8846,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H204" t="inlineStr"/>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H205" t="inlineStr"/>
@@ -8926,7 +8926,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H206" t="inlineStr"/>
@@ -8970,7 +8970,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H207" t="inlineStr"/>
@@ -9010,7 +9010,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H208" t="inlineStr"/>
@@ -9050,7 +9050,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H209" t="inlineStr"/>
@@ -9094,7 +9094,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H210" t="inlineStr"/>
@@ -9134,7 +9134,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H211" t="inlineStr"/>
@@ -9174,7 +9174,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H212" t="inlineStr"/>
@@ -9218,7 +9218,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H213" t="inlineStr"/>
@@ -9258,7 +9258,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H214" t="inlineStr"/>
@@ -9298,7 +9298,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H215" t="inlineStr"/>
@@ -9338,7 +9338,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H216" t="inlineStr"/>
@@ -9382,7 +9382,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H217" t="inlineStr"/>
@@ -9422,7 +9422,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H218" t="inlineStr"/>
@@ -9462,7 +9462,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H219" t="inlineStr"/>
@@ -9502,7 +9502,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H220" t="inlineStr"/>
@@ -9546,7 +9546,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H221" t="inlineStr"/>
@@ -9586,7 +9586,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H222" t="inlineStr"/>
@@ -9626,7 +9626,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H223" t="inlineStr"/>
@@ -9670,7 +9670,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H224" t="inlineStr"/>
@@ -9710,7 +9710,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H225" t="inlineStr"/>
@@ -9750,7 +9750,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H226" t="inlineStr"/>
@@ -9794,7 +9794,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H227" t="inlineStr"/>
@@ -9834,7 +9834,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H228" t="inlineStr"/>
@@ -9874,7 +9874,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H229" t="inlineStr"/>
@@ -9918,7 +9918,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H230" t="inlineStr"/>
@@ -9958,7 +9958,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H231" t="inlineStr"/>
@@ -9998,7 +9998,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H232" t="inlineStr"/>
@@ -10042,7 +10042,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H233" t="inlineStr"/>
@@ -10082,7 +10082,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H234" t="inlineStr"/>
@@ -10122,7 +10122,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H235" t="inlineStr"/>
@@ -10166,7 +10166,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H236" t="inlineStr"/>
@@ -10206,7 +10206,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H237" t="inlineStr"/>
@@ -10246,7 +10246,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H238" t="inlineStr"/>
@@ -10290,7 +10290,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H239" t="inlineStr"/>
@@ -10330,7 +10330,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H240" t="inlineStr"/>
@@ -10370,7 +10370,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H241" t="inlineStr"/>
@@ -10414,7 +10414,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H242" t="inlineStr"/>
@@ -10454,7 +10454,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H243" t="inlineStr"/>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H244" t="inlineStr"/>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H245" t="inlineStr"/>
@@ -10578,7 +10578,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H246" t="inlineStr"/>
@@ -10618,7 +10618,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H247" t="inlineStr"/>
@@ -10662,7 +10662,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H248" t="inlineStr"/>
@@ -10702,7 +10702,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H249" t="inlineStr"/>
@@ -10742,7 +10742,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H250" t="inlineStr"/>
@@ -10786,7 +10786,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H251" t="inlineStr"/>
@@ -10826,7 +10826,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H252" t="inlineStr"/>
@@ -10866,7 +10866,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H253" t="inlineStr"/>
@@ -10910,7 +10910,7 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H254" t="inlineStr"/>
@@ -10950,7 +10950,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H255" t="inlineStr"/>
@@ -10990,7 +10990,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H256" t="inlineStr"/>
@@ -11034,7 +11034,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H257" t="inlineStr"/>
@@ -11074,7 +11074,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H258" t="inlineStr"/>
@@ -11114,7 +11114,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H259" t="inlineStr"/>
@@ -11158,7 +11158,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H260" t="inlineStr"/>
@@ -11198,7 +11198,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H261" t="inlineStr"/>
@@ -11238,7 +11238,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H262" t="inlineStr"/>
@@ -11282,7 +11282,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H263" t="inlineStr"/>
@@ -11322,7 +11322,7 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H264" t="inlineStr"/>
@@ -11362,7 +11362,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H265" t="inlineStr"/>
@@ -11406,7 +11406,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H266" t="inlineStr"/>
@@ -11446,7 +11446,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H267" t="inlineStr"/>
@@ -11486,7 +11486,7 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H268" t="inlineStr"/>
@@ -11530,7 +11530,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H269" t="inlineStr"/>
@@ -11570,7 +11570,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H270" t="inlineStr"/>
@@ -11610,7 +11610,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H271" t="inlineStr"/>
@@ -11654,7 +11654,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H272" t="inlineStr"/>
@@ -11694,7 +11694,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H273" t="inlineStr"/>
@@ -11734,7 +11734,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H274" t="inlineStr"/>
@@ -11778,7 +11778,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H275" t="inlineStr"/>
@@ -11818,7 +11818,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H276" t="inlineStr"/>
@@ -11858,7 +11858,7 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H277" t="inlineStr"/>
@@ -11902,7 +11902,7 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H278" t="inlineStr"/>
@@ -11942,7 +11942,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H279" t="inlineStr"/>
@@ -11982,7 +11982,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H280" t="inlineStr"/>
@@ -12026,7 +12026,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H281" t="inlineStr"/>
@@ -12066,7 +12066,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H282" t="inlineStr"/>
@@ -12106,7 +12106,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H283" t="inlineStr"/>
@@ -12150,7 +12150,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H284" t="inlineStr"/>
@@ -12190,7 +12190,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H285" t="inlineStr"/>
@@ -12230,7 +12230,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H286" t="inlineStr"/>
@@ -12274,7 +12274,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H287" t="inlineStr"/>
@@ -12314,7 +12314,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H288" t="inlineStr"/>
@@ -12354,7 +12354,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H289" t="inlineStr"/>
@@ -12398,7 +12398,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H290" t="inlineStr"/>
@@ -12438,7 +12438,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H291" t="inlineStr"/>
@@ -12478,7 +12478,7 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>phrase</t>
         </is>
       </c>
       <c r="H292" t="inlineStr"/>

</xml_diff>

<commit_message>
Refactor phrase type determination logic
Removed parser-provided type prioritization and unified phrase type determination to use the internal method. Improved infinitive pattern detection to exclude pronouns after 'to'.
</commit_message>
<xml_diff>
--- a/training/data/例文入力元_分解結果_v2.xlsx
+++ b/training/data/例文入力元_分解結果_v2.xlsx
@@ -526,7 +526,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -606,7 +606,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -646,7 +646,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -686,7 +686,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -730,7 +730,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -770,7 +770,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -810,7 +810,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -854,7 +854,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -894,7 +894,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
@@ -934,7 +934,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -978,7 +978,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -1678,7 +1678,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H33" t="inlineStr"/>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H34" t="inlineStr"/>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H36" t="inlineStr"/>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H40" t="inlineStr"/>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H41" t="inlineStr"/>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
@@ -2222,7 +2222,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H43" t="inlineStr"/>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H44" t="inlineStr"/>
@@ -2302,7 +2302,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H45" t="inlineStr"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
@@ -2470,7 +2470,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
@@ -2510,7 +2510,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
@@ -2554,7 +2554,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H51" t="inlineStr"/>
@@ -2594,7 +2594,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H55" t="inlineStr"/>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -2798,7 +2798,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
@@ -3042,7 +3042,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
@@ -3122,7 +3122,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H65" t="inlineStr"/>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
@@ -3326,7 +3326,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
@@ -3534,7 +3534,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
@@ -3618,7 +3618,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
@@ -3658,7 +3658,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
@@ -3742,7 +3742,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
@@ -3906,7 +3906,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
@@ -3946,7 +3946,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
@@ -4070,7 +4070,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
@@ -4190,7 +4190,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
@@ -4274,7 +4274,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
@@ -4354,7 +4354,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
@@ -4478,7 +4478,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
@@ -4518,7 +4518,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
@@ -4558,7 +4558,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
@@ -4598,7 +4598,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H102" t="inlineStr"/>
@@ -4682,7 +4682,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
@@ -4722,7 +4722,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
@@ -4762,7 +4762,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
@@ -4806,7 +4806,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H106" t="inlineStr"/>
@@ -4846,7 +4846,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H107" t="inlineStr"/>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
@@ -4970,7 +4970,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H110" t="inlineStr"/>
@@ -5010,7 +5010,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H111" t="inlineStr"/>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H112" t="inlineStr"/>
@@ -5094,7 +5094,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H113" t="inlineStr"/>
@@ -5134,7 +5134,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H114" t="inlineStr"/>
@@ -5178,7 +5178,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H115" t="inlineStr"/>
@@ -5218,7 +5218,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H116" t="inlineStr"/>
@@ -5258,7 +5258,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H117" t="inlineStr"/>
@@ -5302,7 +5302,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H118" t="inlineStr"/>
@@ -5342,7 +5342,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H119" t="inlineStr"/>
@@ -5382,7 +5382,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H120" t="inlineStr"/>
@@ -5426,7 +5426,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H121" t="inlineStr"/>
@@ -5466,7 +5466,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H122" t="inlineStr"/>
@@ -5506,7 +5506,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H123" t="inlineStr"/>
@@ -5550,7 +5550,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H124" t="inlineStr"/>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H125" t="inlineStr"/>
@@ -5630,7 +5630,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H126" t="inlineStr"/>
@@ -5674,7 +5674,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H127" t="inlineStr"/>
@@ -5714,7 +5714,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H128" t="inlineStr"/>
@@ -5754,7 +5754,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H129" t="inlineStr"/>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H130" t="inlineStr"/>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H131" t="inlineStr"/>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H132" t="inlineStr"/>
@@ -5918,7 +5918,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H133" t="inlineStr"/>
@@ -5958,7 +5958,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H134" t="inlineStr"/>
@@ -5998,7 +5998,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H135" t="inlineStr"/>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H136" t="inlineStr"/>
@@ -6082,7 +6082,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H137" t="inlineStr"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H138" t="inlineStr"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H139" t="inlineStr"/>
@@ -6202,7 +6202,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H140" t="inlineStr"/>
@@ -6242,7 +6242,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H141" t="inlineStr"/>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H142" t="inlineStr"/>
@@ -6326,7 +6326,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H143" t="inlineStr"/>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H144" t="inlineStr"/>
@@ -6406,7 +6406,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H145" t="inlineStr"/>
@@ -6446,7 +6446,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H146" t="inlineStr"/>
@@ -6490,7 +6490,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H147" t="inlineStr"/>
@@ -6530,7 +6530,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H148" t="inlineStr"/>
@@ -6570,7 +6570,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H149" t="inlineStr"/>
@@ -6614,7 +6614,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H150" t="inlineStr"/>
@@ -6654,7 +6654,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H151" t="inlineStr"/>
@@ -6694,7 +6694,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H152" t="inlineStr"/>
@@ -6738,7 +6738,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H153" t="inlineStr"/>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H154" t="inlineStr"/>
@@ -6818,7 +6818,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H155" t="inlineStr"/>
@@ -6862,7 +6862,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H156" t="inlineStr"/>
@@ -6902,7 +6902,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H157" t="inlineStr"/>
@@ -6942,7 +6942,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H158" t="inlineStr"/>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H159" t="inlineStr"/>
@@ -7026,7 +7026,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H160" t="inlineStr"/>
@@ -7066,7 +7066,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H161" t="inlineStr"/>
@@ -7110,7 +7110,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H162" t="inlineStr"/>
@@ -7150,7 +7150,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H163" t="inlineStr"/>
@@ -7190,7 +7190,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H164" t="inlineStr"/>
@@ -7234,7 +7234,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H165" t="inlineStr"/>
@@ -7274,7 +7274,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H166" t="inlineStr"/>
@@ -7314,7 +7314,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H167" t="inlineStr"/>
@@ -7358,7 +7358,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H168" t="inlineStr"/>
@@ -7398,7 +7398,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H169" t="inlineStr"/>
@@ -7438,7 +7438,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H170" t="inlineStr"/>
@@ -7482,7 +7482,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H171" t="inlineStr"/>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H172" t="inlineStr"/>
@@ -7562,7 +7562,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H173" t="inlineStr"/>
@@ -7606,7 +7606,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H174" t="inlineStr"/>
@@ -7646,7 +7646,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H175" t="inlineStr"/>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H176" t="inlineStr"/>
@@ -7730,7 +7730,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H177" t="inlineStr"/>
@@ -7770,7 +7770,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H178" t="inlineStr"/>
@@ -7810,7 +7810,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H179" t="inlineStr"/>
@@ -7854,7 +7854,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H180" t="inlineStr"/>
@@ -7894,7 +7894,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H181" t="inlineStr"/>
@@ -7934,7 +7934,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H182" t="inlineStr"/>
@@ -7978,7 +7978,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H183" t="inlineStr"/>
@@ -8018,7 +8018,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H184" t="inlineStr"/>
@@ -8058,7 +8058,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H185" t="inlineStr"/>
@@ -8102,7 +8102,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H186" t="inlineStr"/>
@@ -8142,7 +8142,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H187" t="inlineStr"/>
@@ -8182,7 +8182,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H188" t="inlineStr"/>
@@ -8226,7 +8226,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H189" t="inlineStr"/>
@@ -8266,7 +8266,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H190" t="inlineStr"/>
@@ -8306,7 +8306,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H191" t="inlineStr"/>
@@ -8350,7 +8350,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H192" t="inlineStr"/>
@@ -8390,7 +8390,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H193" t="inlineStr"/>
@@ -8430,7 +8430,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H194" t="inlineStr"/>
@@ -8474,7 +8474,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H195" t="inlineStr"/>
@@ -8514,7 +8514,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H196" t="inlineStr"/>
@@ -8554,7 +8554,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H197" t="inlineStr"/>
@@ -8598,7 +8598,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H198" t="inlineStr"/>
@@ -8638,7 +8638,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H199" t="inlineStr"/>
@@ -8678,7 +8678,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H200" t="inlineStr"/>
@@ -8722,7 +8722,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H201" t="inlineStr"/>
@@ -8762,7 +8762,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H202" t="inlineStr"/>
@@ -8802,7 +8802,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H203" t="inlineStr"/>
@@ -8846,7 +8846,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H204" t="inlineStr"/>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H205" t="inlineStr"/>
@@ -8926,7 +8926,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H206" t="inlineStr"/>
@@ -8970,7 +8970,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H207" t="inlineStr"/>
@@ -9010,7 +9010,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H208" t="inlineStr"/>
@@ -9050,7 +9050,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H209" t="inlineStr"/>
@@ -9094,7 +9094,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H210" t="inlineStr"/>
@@ -9134,7 +9134,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H211" t="inlineStr"/>
@@ -9174,7 +9174,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H212" t="inlineStr"/>
@@ -9218,7 +9218,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H213" t="inlineStr"/>
@@ -9258,7 +9258,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H214" t="inlineStr"/>
@@ -9298,7 +9298,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H215" t="inlineStr"/>
@@ -9338,7 +9338,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H216" t="inlineStr"/>
@@ -9382,7 +9382,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H217" t="inlineStr"/>
@@ -9422,7 +9422,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H218" t="inlineStr"/>
@@ -9462,7 +9462,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H219" t="inlineStr"/>
@@ -9502,7 +9502,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H220" t="inlineStr"/>
@@ -9546,7 +9546,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H221" t="inlineStr"/>
@@ -9586,7 +9586,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H222" t="inlineStr"/>
@@ -9626,7 +9626,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H223" t="inlineStr"/>
@@ -9670,7 +9670,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H224" t="inlineStr"/>
@@ -9710,7 +9710,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H225" t="inlineStr"/>
@@ -9750,7 +9750,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H226" t="inlineStr"/>
@@ -9794,7 +9794,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H227" t="inlineStr"/>
@@ -9834,7 +9834,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H228" t="inlineStr"/>
@@ -9874,7 +9874,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H229" t="inlineStr"/>
@@ -9918,7 +9918,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H230" t="inlineStr"/>
@@ -9958,7 +9958,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H231" t="inlineStr"/>
@@ -9998,7 +9998,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H232" t="inlineStr"/>
@@ -10042,7 +10042,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H233" t="inlineStr"/>
@@ -10082,7 +10082,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H234" t="inlineStr"/>
@@ -10122,7 +10122,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H235" t="inlineStr"/>
@@ -10166,7 +10166,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H236" t="inlineStr"/>
@@ -10206,7 +10206,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H237" t="inlineStr"/>
@@ -10246,7 +10246,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H238" t="inlineStr"/>
@@ -10290,7 +10290,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H239" t="inlineStr"/>
@@ -10330,7 +10330,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H240" t="inlineStr"/>
@@ -10370,7 +10370,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H241" t="inlineStr"/>
@@ -10414,7 +10414,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H242" t="inlineStr"/>
@@ -10454,7 +10454,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H243" t="inlineStr"/>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H244" t="inlineStr"/>
@@ -10538,7 +10538,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H245" t="inlineStr"/>
@@ -10578,7 +10578,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H246" t="inlineStr"/>
@@ -10618,7 +10618,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H247" t="inlineStr"/>
@@ -10662,7 +10662,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H248" t="inlineStr"/>
@@ -10702,7 +10702,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H249" t="inlineStr"/>
@@ -10742,7 +10742,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H250" t="inlineStr"/>
@@ -10786,7 +10786,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H251" t="inlineStr"/>
@@ -10826,7 +10826,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H252" t="inlineStr"/>
@@ -10866,7 +10866,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H253" t="inlineStr"/>
@@ -10910,7 +10910,7 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H254" t="inlineStr"/>
@@ -10950,7 +10950,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H255" t="inlineStr"/>
@@ -10990,7 +10990,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H256" t="inlineStr"/>
@@ -11034,7 +11034,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H257" t="inlineStr"/>
@@ -11074,7 +11074,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H258" t="inlineStr"/>
@@ -11114,7 +11114,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H259" t="inlineStr"/>
@@ -11158,7 +11158,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H260" t="inlineStr"/>
@@ -11198,7 +11198,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H261" t="inlineStr"/>
@@ -11238,7 +11238,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H262" t="inlineStr"/>
@@ -11282,7 +11282,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H263" t="inlineStr"/>
@@ -11322,7 +11322,7 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H264" t="inlineStr"/>
@@ -11362,7 +11362,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H265" t="inlineStr"/>
@@ -11406,7 +11406,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H266" t="inlineStr"/>
@@ -11446,7 +11446,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H267" t="inlineStr"/>
@@ -11486,7 +11486,7 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H268" t="inlineStr"/>
@@ -11530,7 +11530,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H269" t="inlineStr"/>
@@ -11570,7 +11570,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H270" t="inlineStr"/>
@@ -11610,7 +11610,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H271" t="inlineStr"/>
@@ -11654,7 +11654,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H272" t="inlineStr"/>
@@ -11694,7 +11694,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H273" t="inlineStr"/>
@@ -11734,7 +11734,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H274" t="inlineStr"/>
@@ -11778,7 +11778,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H275" t="inlineStr"/>
@@ -11818,7 +11818,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H276" t="inlineStr"/>
@@ -11858,7 +11858,7 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H277" t="inlineStr"/>
@@ -11902,7 +11902,7 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H278" t="inlineStr"/>
@@ -11942,7 +11942,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H279" t="inlineStr"/>
@@ -11982,7 +11982,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H280" t="inlineStr"/>
@@ -12026,7 +12026,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H281" t="inlineStr"/>
@@ -12066,7 +12066,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H282" t="inlineStr"/>
@@ -12106,7 +12106,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H283" t="inlineStr"/>
@@ -12150,7 +12150,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H284" t="inlineStr"/>
@@ -12190,7 +12190,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H285" t="inlineStr"/>
@@ -12230,7 +12230,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H286" t="inlineStr"/>
@@ -12274,7 +12274,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H287" t="inlineStr"/>
@@ -12314,7 +12314,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H288" t="inlineStr"/>
@@ -12354,7 +12354,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H289" t="inlineStr"/>
@@ -12398,7 +12398,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H290" t="inlineStr"/>
@@ -12438,7 +12438,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H291" t="inlineStr"/>
@@ -12478,7 +12478,7 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H292" t="inlineStr"/>

</xml_diff>

<commit_message>
Update training data Excel file
Replaced the existing training data Excel file with a new version to reflect updated or corrected data.
</commit_message>
<xml_diff>
--- a/training/data/例文入力元_分解結果_v2.xlsx
+++ b/training/data/例文入力元_分解結果_v2.xlsx
@@ -770,7 +770,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -8134,7 +8134,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H187" t="inlineStr"/>
@@ -9818,7 +9818,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H228" t="inlineStr"/>
@@ -10978,7 +10978,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H256" t="inlineStr"/>
@@ -11062,7 +11062,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H258" t="inlineStr"/>
@@ -11146,7 +11146,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H260" t="inlineStr"/>
@@ -11230,7 +11230,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>phrase</t>
+          <t>word</t>
         </is>
       </c>
       <c r="H262" t="inlineStr"/>

</xml_diff>